<commit_message>
debugging the sensitivity analysis
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_SA.xlsx
+++ b/data/Czech/KCOR_SA.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,7 +599,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2021_24</t>
+          <t xml:space="preserve">2021_24,2022_06   </t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t xml:space="preserve">0   </t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2021_24</t>
+          <t xml:space="preserve">2021_24,2022_06   </t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -683,7 +683,155 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022_06</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.118634762881549</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.071698934433147</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.167626179817872</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>92</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24,2022_06   </t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022_06</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.060430986706911</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.037039328387625</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.084350271765076</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>92</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24,2022_06   </t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated makefile with additional parameters for the sensitivity tests
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_SA.xlsx
+++ b/data/Czech/KCOR_SA.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,13 +558,13 @@
         <v>44921</v>
       </c>
       <c r="F2" t="n">
-        <v>1.054174388061531</v>
+        <v>1.100394261025673</v>
       </c>
       <c r="G2" t="n">
-        <v>1.02474732932989</v>
+        <v>1.069913537801219</v>
       </c>
       <c r="H2" t="n">
-        <v>1.084446486112437</v>
+        <v>1.131743348333261</v>
       </c>
       <c r="I2" t="n">
         <v>4</v>
@@ -595,7 +595,7 @@
         <v>50</v>
       </c>
       <c r="Q2" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -632,13 +632,13 @@
         <v>44921</v>
       </c>
       <c r="F3" t="n">
-        <v>1.052397545338201</v>
+        <v>1.060120547301205</v>
       </c>
       <c r="G3" t="n">
-        <v>1.023038305836997</v>
+        <v>1.030538283130707</v>
       </c>
       <c r="H3" t="n">
-        <v>1.082599338768393</v>
+        <v>1.090551989389475</v>
       </c>
       <c r="I3" t="n">
         <v>4</v>
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -706,13 +706,13 @@
         <v>44921</v>
       </c>
       <c r="F4" t="n">
-        <v>1.031486777250451</v>
+        <v>1.056796329578352</v>
       </c>
       <c r="G4" t="n">
-        <v>1.002718944492117</v>
+        <v>1.027643832100711</v>
       </c>
       <c r="H4" t="n">
-        <v>1.061079954145503</v>
+        <v>1.086775833536874</v>
       </c>
       <c r="I4" t="n">
         <v>4</v>
@@ -740,10 +740,10 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q4" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -780,13 +780,13 @@
         <v>44921</v>
       </c>
       <c r="F5" t="n">
-        <v>1.029697355259162</v>
+        <v>1.028005378998235</v>
       </c>
       <c r="G5" t="n">
-        <v>1.001013952810909</v>
+        <v>0.9993050529201893</v>
       </c>
       <c r="H5" t="n">
-        <v>1.059202661911347</v>
+        <v>1.057529986625322</v>
       </c>
       <c r="I5" t="n">
         <v>4</v>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="Q5" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -854,13 +854,13 @@
         <v>44921</v>
       </c>
       <c r="F6" t="n">
-        <v>1.03662292202496</v>
+        <v>1.056436123388405</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0077615353228</v>
+        <v>1.0271348823065</v>
       </c>
       <c r="H6" t="n">
-        <v>1.066310872961986</v>
+        <v>1.086573245661505</v>
       </c>
       <c r="I6" t="n">
         <v>4</v>
@@ -888,10 +888,10 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
@@ -928,13 +928,13 @@
         <v>44921</v>
       </c>
       <c r="F7" t="n">
-        <v>1.05186124792484</v>
+        <v>1.032707690232421</v>
       </c>
       <c r="G7" t="n">
-        <v>1.022569719623564</v>
+        <v>1.003868826910049</v>
       </c>
       <c r="H7" t="n">
-        <v>1.081991832589472</v>
+        <v>1.062375028366873</v>
       </c>
       <c r="I7" t="n">
         <v>4</v>
@@ -962,10 +962,10 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="Q7" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
@@ -1002,13 +1002,13 @@
         <v>44921</v>
       </c>
       <c r="F8" t="n">
-        <v>1.069794542350042</v>
+        <v>1.089176533026487</v>
       </c>
       <c r="G8" t="n">
-        <v>1.039988170937004</v>
+        <v>1.058866420352971</v>
       </c>
       <c r="H8" t="n">
-        <v>1.100455173264909</v>
+        <v>1.120354274432602</v>
       </c>
       <c r="I8" t="n">
         <v>4</v>
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Q8" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1076,13 +1076,13 @@
         <v>44921</v>
       </c>
       <c r="F9" t="n">
-        <v>1.070650913744666</v>
+        <v>1.054084923747426</v>
       </c>
       <c r="G9" t="n">
-        <v>1.040736224616306</v>
+        <v>1.024649819411033</v>
       </c>
       <c r="H9" t="n">
-        <v>1.101425464002561</v>
+        <v>1.084365610009352</v>
       </c>
       <c r="I9" t="n">
         <v>4</v>
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="Q9" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
@@ -1150,13 +1150,13 @@
         <v>44921</v>
       </c>
       <c r="F10" t="n">
-        <v>1.069087206739409</v>
+        <v>1.144874480900621</v>
       </c>
       <c r="G10" t="n">
-        <v>1.039162305317119</v>
+        <v>1.112879919671963</v>
       </c>
       <c r="H10" t="n">
-        <v>1.099873859709606</v>
+        <v>1.17778886459181</v>
       </c>
       <c r="I10" t="n">
         <v>4</v>
@@ -1184,10 +1184,10 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="Q10" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R10" t="inlineStr">
         <is>
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1224,13 +1224,13 @@
         <v>44921</v>
       </c>
       <c r="F11" t="n">
-        <v>1.265599914753201</v>
+        <v>1.043400007471209</v>
       </c>
       <c r="G11" t="n">
-        <v>1.239212015350355</v>
+        <v>1.014291607573952</v>
       </c>
       <c r="H11" t="n">
-        <v>1.292549720614562</v>
+        <v>1.073343767671412</v>
       </c>
       <c r="I11" t="n">
         <v>4</v>
@@ -1258,10 +1258,10 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="Q11" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -1298,13 +1298,13 @@
         <v>44921</v>
       </c>
       <c r="F12" t="n">
-        <v>1.262608901748548</v>
+        <v>1.063626313435</v>
       </c>
       <c r="G12" t="n">
-        <v>1.236287534282729</v>
+        <v>1.03377789605819</v>
       </c>
       <c r="H12" t="n">
-        <v>1.289490668285018</v>
+        <v>1.094336548445266</v>
       </c>
       <c r="I12" t="n">
         <v>4</v>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="Q12" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R12" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -1372,13 +1372,13 @@
         <v>44921</v>
       </c>
       <c r="F13" t="n">
-        <v>1.302239077010254</v>
+        <v>1.049379303316326</v>
       </c>
       <c r="G13" t="n">
-        <v>1.275085321682028</v>
+        <v>1.020123826282271</v>
       </c>
       <c r="H13" t="n">
-        <v>1.329971088880131</v>
+        <v>1.079473779415435</v>
       </c>
       <c r="I13" t="n">
         <v>4</v>
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="Q13" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1446,13 +1446,13 @@
         <v>44921</v>
       </c>
       <c r="F14" t="n">
-        <v>1.321532763154709</v>
+        <v>1.104965610402203</v>
       </c>
       <c r="G14" t="n">
-        <v>1.293989658925252</v>
+        <v>1.073742600267662</v>
       </c>
       <c r="H14" t="n">
-        <v>1.349662133731321</v>
+        <v>1.137096544243616</v>
       </c>
       <c r="I14" t="n">
         <v>4</v>
@@ -1480,10 +1480,10 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="Q14" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R14" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -1520,13 +1520,13 @@
         <v>44921</v>
       </c>
       <c r="F15" t="n">
-        <v>1.300260015281328</v>
+        <v>1.076415427293776</v>
       </c>
       <c r="G15" t="n">
-        <v>1.273173032693385</v>
+        <v>1.046338394497358</v>
       </c>
       <c r="H15" t="n">
-        <v>1.327923278238771</v>
+        <v>1.107357025422589</v>
       </c>
       <c r="I15" t="n">
         <v>4</v>
@@ -1554,10 +1554,10 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="Q15" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R15" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -1594,13 +1594,13 @@
         <v>44921</v>
       </c>
       <c r="F16" t="n">
-        <v>1.308412736323576</v>
+        <v>1.149895234655831</v>
       </c>
       <c r="G16" t="n">
-        <v>1.28116711469674</v>
+        <v>1.117523759939215</v>
       </c>
       <c r="H16" t="n">
-        <v>1.336237770182678</v>
+        <v>1.183204418630088</v>
       </c>
       <c r="I16" t="n">
         <v>4</v>
@@ -1628,10 +1628,10 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="Q16" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R16" t="inlineStr">
         <is>
@@ -1656,7 +1656,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1668,13 +1668,13 @@
         <v>44921</v>
       </c>
       <c r="F17" t="n">
-        <v>1.333837220883271</v>
+        <v>1.09987679786062</v>
       </c>
       <c r="G17" t="n">
-        <v>1.306056401805583</v>
+        <v>1.06918785736751</v>
       </c>
       <c r="H17" t="n">
-        <v>1.362208959240985</v>
+        <v>1.131446604201673</v>
       </c>
       <c r="I17" t="n">
         <v>4</v>
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="Q17" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R17" t="inlineStr">
         <is>
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -1742,13 +1742,13 @@
         <v>44921</v>
       </c>
       <c r="F18" t="n">
-        <v>1.315545195109145</v>
+        <v>1.142066776644488</v>
       </c>
       <c r="G18" t="n">
-        <v>1.288079213018227</v>
+        <v>1.110047580377162</v>
       </c>
       <c r="H18" t="n">
-        <v>1.343596840072808</v>
+        <v>1.175009562988248</v>
       </c>
       <c r="I18" t="n">
         <v>4</v>
@@ -1776,10 +1776,10 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="Q18" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="R18" t="inlineStr">
         <is>
@@ -1804,7 +1804,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -1816,13 +1816,13 @@
         <v>44921</v>
       </c>
       <c r="F19" t="n">
-        <v>1.303555887444382</v>
+        <v>1.089472389779502</v>
       </c>
       <c r="G19" t="n">
-        <v>1.276298990588932</v>
+        <v>1.059062711668649</v>
       </c>
       <c r="H19" t="n">
-        <v>1.331394888047987</v>
+        <v>1.120755244249618</v>
       </c>
       <c r="I19" t="n">
         <v>4</v>
@@ -1850,10 +1850,10 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="Q19" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R19" t="inlineStr">
         <is>
@@ -1866,6 +1866,1338 @@
         </is>
       </c>
       <c r="T19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.25757019407007</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.231539612373409</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.284150974214804</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4</v>
+      </c>
+      <c r="J20" t="n">
+        <v>8</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>26</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.281336271840238</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.254618150744643</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.308623377207625</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>8</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>2</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>52</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.285939610516232</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.259385400261202</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.313053717751267</v>
+      </c>
+      <c r="I22" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" t="n">
+        <v>8</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>26</v>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.265268453446546</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.23887720187076</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.29222190614984</v>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>8</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>52</v>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.276041989803972</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.249537775447347</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.303108390748682</v>
+      </c>
+      <c r="I24" t="n">
+        <v>4</v>
+      </c>
+      <c r="J24" t="n">
+        <v>8</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>2</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P24" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>26</v>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.268887462429824</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.242402940540979</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.295936559527559</v>
+      </c>
+      <c r="I25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J25" t="n">
+        <v>8</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>2</v>
+      </c>
+      <c r="M25" t="n">
+        <v>1</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>52</v>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.223635513572205</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.19813152438739</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.249682392624367</v>
+      </c>
+      <c r="I26" t="n">
+        <v>4</v>
+      </c>
+      <c r="J26" t="n">
+        <v>8</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>2</v>
+      </c>
+      <c r="M26" t="n">
+        <v>1</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>26</v>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.274882736331023</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.248261863643569</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.302071335136915</v>
+      </c>
+      <c r="I27" t="n">
+        <v>4</v>
+      </c>
+      <c r="J27" t="n">
+        <v>8</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>52</v>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.193579363647159</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.168619199929998</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.219072643517833</v>
+      </c>
+      <c r="I28" t="n">
+        <v>4</v>
+      </c>
+      <c r="J28" t="n">
+        <v>8</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" t="n">
+        <v>2</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P28" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>26</v>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.298412772635451</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.271310252848945</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.32609307945477</v>
+      </c>
+      <c r="I29" t="n">
+        <v>4</v>
+      </c>
+      <c r="J29" t="n">
+        <v>8</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P29" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>52</v>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1.333861274005588</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.30587572742199</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.362446564348211</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4</v>
+      </c>
+      <c r="J30" t="n">
+        <v>8</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P30" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>26</v>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1.340787193043524</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.312833788027927</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.369335793626978</v>
+      </c>
+      <c r="I31" t="n">
+        <v>4</v>
+      </c>
+      <c r="J31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P31" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>52</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1.334525834714396</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.306393579633989</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.363263897866925</v>
+      </c>
+      <c r="I32" t="n">
+        <v>4</v>
+      </c>
+      <c r="J32" t="n">
+        <v>8</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>2</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>26</v>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1.342538475001166</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1.31451631107186</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.371158000609948</v>
+      </c>
+      <c r="I33" t="n">
+        <v>4</v>
+      </c>
+      <c r="J33" t="n">
+        <v>8</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>2</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P33" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>52</v>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1.340461352011904</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.312313185812529</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.369213275964348</v>
+      </c>
+      <c r="I34" t="n">
+        <v>4</v>
+      </c>
+      <c r="J34" t="n">
+        <v>8</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>2</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P34" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>26</v>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.338089852649773</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.310195563445421</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1.366578016075596</v>
+      </c>
+      <c r="I35" t="n">
+        <v>4</v>
+      </c>
+      <c r="J35" t="n">
+        <v>8</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>2</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P35" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>52</v>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.391060184134828</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.361946018191876</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1.420796720309222</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4</v>
+      </c>
+      <c r="J36" t="n">
+        <v>8</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P36" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>26</v>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0   </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2021_24</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>44921</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.332565208984152</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.304776005555133</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1.360946268658175</v>
+      </c>
+      <c r="I37" t="n">
+        <v>4</v>
+      </c>
+      <c r="J37" t="n">
+        <v>8</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" t="n">
+        <v>2</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>4/1/24</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>52</v>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2021_24 </t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>1,0;2,0</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
         <is>
           <t xml:space="preserve">0   </t>
         </is>

</xml_diff>